<commit_message>
mark columns that have been processed
</commit_message>
<xml_diff>
--- a/design/players_table_schema.xlsx
+++ b/design/players_table_schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP USER\Documents\repos\nhl_draft\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D8039B-F0B2-40B5-8848-F5030AEA724E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43651AC6-4278-49FF-8DFC-4B19151A2E6B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22224" windowHeight="13176" xr2:uid="{04C11591-E26B-41C8-AB0B-0A429CAB3277}"/>
   </bookViews>
@@ -625,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8CB7A3C-C098-4C7D-82B8-C06EACCEF5D2}">
   <dimension ref="A1:AA6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -721,10 +721,10 @@
       <c r="S2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="T2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="U2" s="5" t="s">
         <v>53</v>
       </c>
       <c r="V2" s="2" t="s">

</xml_diff>